<commit_message>
updated pol grade selection criteria
</commit_message>
<xml_diff>
--- a/cec_clay_susc.xlsx
+++ b/cec_clay_susc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/gaston_mendozaveirana_ugent_be/Documents/Documentos/PhD/Magnetics/Magnetism_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="686" documentId="13_ncr:1_{8ABC0D2B-C8E5-44D1-926B-ADB09F951735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{007492A0-1494-427B-BC22-69D129FDFAAA}"/>
+  <xr:revisionPtr revIDLastSave="687" documentId="13_ncr:1_{8ABC0D2B-C8E5-44D1-926B-ADB09F951735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2513B038-4A4A-47CE-9FB9-A1D275004262}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1752,7 +1752,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1973,40 +1973,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EF183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="11" ySplit="12" topLeftCell="DM171" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="DP2" sqref="DP2"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="DP2" sqref="DP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" customWidth="1"/>
-    <col min="11" max="18" width="9.140625" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="11" max="18" width="9.109375" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" customWidth="1"/>
     <col min="21" max="21" width="12" customWidth="1"/>
-    <col min="22" max="117" width="9.140625" customWidth="1"/>
-    <col min="122" max="122" width="11.5703125" customWidth="1"/>
-    <col min="123" max="123" width="10.85546875" customWidth="1"/>
-    <col min="124" max="124" width="10.42578125" customWidth="1"/>
-    <col min="125" max="125" width="10.5703125" customWidth="1"/>
-    <col min="126" max="127" width="10.42578125" customWidth="1"/>
-    <col min="129" max="129" width="10.140625" customWidth="1"/>
+    <col min="22" max="117" width="9.109375" customWidth="1"/>
+    <col min="122" max="122" width="11.5546875" customWidth="1"/>
+    <col min="123" max="123" width="10.88671875" customWidth="1"/>
+    <col min="124" max="124" width="10.44140625" customWidth="1"/>
+    <col min="125" max="125" width="10.5546875" customWidth="1"/>
+    <col min="126" max="127" width="10.44140625" customWidth="1"/>
+    <col min="129" max="129" width="10.109375" customWidth="1"/>
     <col min="130" max="130" width="11" customWidth="1"/>
-    <col min="131" max="131" width="10.85546875" customWidth="1"/>
-    <col min="132" max="132" width="10.42578125" customWidth="1"/>
-    <col min="134" max="134" width="9.7109375" customWidth="1"/>
-    <col min="135" max="136" width="10.42578125" customWidth="1"/>
+    <col min="131" max="131" width="10.88671875" customWidth="1"/>
+    <col min="132" max="132" width="10.44140625" customWidth="1"/>
+    <col min="134" max="134" width="9.6640625" customWidth="1"/>
+    <col min="135" max="136" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2416,7 +2413,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>108</v>
       </c>
@@ -2826,7 +2823,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="3" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -3236,7 +3233,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="4" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>115</v>
       </c>
@@ -3646,7 +3643,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="5" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>118</v>
       </c>
@@ -4056,7 +4053,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="6" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>121</v>
       </c>
@@ -4466,7 +4463,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="7" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -4876,7 +4873,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="8" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>127</v>
       </c>
@@ -5286,7 +5283,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="9" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>130</v>
       </c>
@@ -5696,7 +5693,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="10" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>133</v>
       </c>
@@ -6106,7 +6103,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="11" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>136</v>
       </c>
@@ -6516,7 +6513,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="12" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>139</v>
       </c>
@@ -6926,7 +6923,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="13" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>142</v>
       </c>
@@ -7336,7 +7333,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="14" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>145</v>
       </c>
@@ -7746,7 +7743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>148</v>
       </c>
@@ -8156,7 +8153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>151</v>
       </c>
@@ -8566,7 +8563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>154</v>
       </c>
@@ -8976,7 +8973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>157</v>
       </c>
@@ -9386,7 +9383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
@@ -9796,7 +9793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>163</v>
       </c>
@@ -10206,7 +10203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>166</v>
       </c>
@@ -10616,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:136" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>170</v>
       </c>
@@ -11026,7 +11023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>173</v>
       </c>
@@ -11436,7 +11433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>176</v>
       </c>
@@ -11846,7 +11843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>487</v>
       </c>
@@ -12259,7 +12256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>488</v>
       </c>
@@ -12672,7 +12669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>489</v>
       </c>
@@ -13085,7 +13082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>490</v>
       </c>
@@ -13498,7 +13495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>491</v>
       </c>
@@ -13911,7 +13908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>194</v>
       </c>
@@ -14324,7 +14321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>197</v>
       </c>
@@ -14737,7 +14734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>200</v>
       </c>
@@ -15150,7 +15147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>203</v>
       </c>
@@ -15563,7 +15560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>206</v>
       </c>
@@ -15976,7 +15973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>209</v>
       </c>
@@ -16389,7 +16386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>482</v>
       </c>
@@ -16802,7 +16799,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="37" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>483</v>
       </c>
@@ -17215,7 +17212,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="38" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>484</v>
       </c>
@@ -17628,7 +17625,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="39" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>485</v>
       </c>
@@ -18041,7 +18038,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="40" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>486</v>
       </c>
@@ -18454,7 +18451,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="41" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>358</v>
       </c>
@@ -18867,7 +18864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>359</v>
       </c>
@@ -19280,7 +19277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>360</v>
       </c>
@@ -19693,7 +19690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -20106,7 +20103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>362</v>
       </c>
@@ -20519,7 +20516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>232</v>
       </c>
@@ -20932,7 +20929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>235</v>
       </c>
@@ -21345,7 +21342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>238</v>
       </c>
@@ -21758,7 +21755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>241</v>
       </c>
@@ -22171,7 +22168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>244</v>
       </c>
@@ -22584,7 +22581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>247</v>
       </c>
@@ -22997,7 +22994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>250</v>
       </c>
@@ -23410,7 +23407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="s">
         <v>253</v>
       </c>
@@ -23823,7 +23820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
         <v>256</v>
       </c>
@@ -24236,7 +24233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19" t="s">
         <v>259</v>
       </c>
@@ -24649,7 +24646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>262</v>
       </c>
@@ -25062,7 +25059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:136" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19" t="s">
         <v>265</v>
       </c>
@@ -25475,7 +25472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>363</v>
       </c>
@@ -25553,7 +25550,7 @@
         <v>53.5</v>
       </c>
     </row>
-    <row r="59" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>364</v>
       </c>
@@ -25631,7 +25628,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>365</v>
       </c>
@@ -25709,7 +25706,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="61" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>366</v>
       </c>
@@ -25787,7 +25784,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>367</v>
       </c>
@@ -25865,7 +25862,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="63" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>368</v>
       </c>
@@ -25943,7 +25940,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="64" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>369</v>
       </c>
@@ -26018,7 +26015,7 @@
         <v>-4.2556631378829479E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>370</v>
       </c>
@@ -26093,7 +26090,7 @@
         <v>-4.2370326817035675E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>371</v>
       </c>
@@ -26168,7 +26165,7 @@
         <v>-8.8877856731414795E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>372</v>
       </c>
@@ -26243,7 +26240,7 @@
         <v>-3.7703100591897964E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>373</v>
       </c>
@@ -26321,7 +26318,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="69" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>374</v>
       </c>
@@ -26399,7 +26396,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="70" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>375</v>
       </c>
@@ -26477,7 +26474,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:136" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:136" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="32" t="s">
         <v>378</v>
       </c>
@@ -26551,7 +26548,7 @@
         <v>0.27946656942367554</v>
       </c>
     </row>
-    <row r="72" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="32" t="s">
         <v>379</v>
       </c>
@@ -26628,7 +26625,7 @@
         <v>0.37572139501571655</v>
       </c>
     </row>
-    <row r="73" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="32" t="s">
         <v>380</v>
       </c>
@@ -26705,7 +26702,7 @@
         <v>0.30379319190979004</v>
       </c>
     </row>
-    <row r="74" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="32" t="s">
         <v>381</v>
       </c>
@@ -26782,7 +26779,7 @@
         <v>0.28026676177978516</v>
       </c>
     </row>
-    <row r="75" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="32" t="s">
         <v>382</v>
       </c>
@@ -26859,7 +26856,7 @@
         <v>0.21553769707679749</v>
       </c>
     </row>
-    <row r="76" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="32" t="s">
         <v>383</v>
       </c>
@@ -26936,7 +26933,7 @@
         <v>0.35205289721488953</v>
       </c>
     </row>
-    <row r="77" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="32" t="s">
         <v>384</v>
       </c>
@@ -27013,7 +27010,7 @@
         <v>0.26276829838752747</v>
       </c>
     </row>
-    <row r="78" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="32" t="s">
         <v>385</v>
       </c>
@@ -27090,7 +27087,7 @@
         <v>0.21474047005176544</v>
       </c>
     </row>
-    <row r="79" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="32" t="s">
         <v>386</v>
       </c>
@@ -27167,7 +27164,7 @@
         <v>0.24467624723911285</v>
       </c>
     </row>
-    <row r="80" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="32" t="s">
         <v>387</v>
       </c>
@@ -27244,7 +27241,7 @@
         <v>0.23062732815742493</v>
       </c>
     </row>
-    <row r="81" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="32" t="s">
         <v>388</v>
       </c>
@@ -27321,7 +27318,7 @@
         <v>0.37819677591323853</v>
       </c>
     </row>
-    <row r="82" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="32" t="s">
         <v>389</v>
       </c>
@@ -27398,7 +27395,7 @@
         <v>0.15000160038471222</v>
       </c>
     </row>
-    <row r="83" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="32" t="s">
         <v>390</v>
       </c>
@@ -27475,7 +27472,7 @@
         <v>0.15553762018680573</v>
       </c>
     </row>
-    <row r="84" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="32" t="s">
         <v>391</v>
       </c>
@@ -27552,7 +27549,7 @@
         <v>0.14689597487449646</v>
       </c>
     </row>
-    <row r="85" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="32" t="s">
         <v>392</v>
       </c>
@@ -27629,7 +27626,7 @@
         <v>0.15037035942077637</v>
       </c>
     </row>
-    <row r="86" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="32" t="s">
         <v>393</v>
       </c>
@@ -27706,7 +27703,7 @@
         <v>0.19597060978412628</v>
       </c>
     </row>
-    <row r="87" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="32" t="s">
         <v>394</v>
       </c>
@@ -27783,7 +27780,7 @@
         <v>0.21237118542194366</v>
       </c>
     </row>
-    <row r="88" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="32" t="s">
         <v>395</v>
       </c>
@@ -27860,7 +27857,7 @@
         <v>0.27280253171920776</v>
       </c>
     </row>
-    <row r="89" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="32" t="s">
         <v>396</v>
       </c>
@@ -27937,7 +27934,7 @@
         <v>0.25055074691772461</v>
       </c>
     </row>
-    <row r="90" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="32" t="s">
         <v>397</v>
       </c>
@@ -28014,7 +28011,7 @@
         <v>0.26519650220870972</v>
       </c>
     </row>
-    <row r="91" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="32" t="s">
         <v>398</v>
       </c>
@@ -28091,7 +28088,7 @@
         <v>0.3914719820022583</v>
       </c>
     </row>
-    <row r="92" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
         <v>399</v>
       </c>
@@ -28168,7 +28165,7 @@
         <v>0.43903306126594543</v>
       </c>
     </row>
-    <row r="93" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
         <v>400</v>
       </c>
@@ -28245,7 +28242,7 @@
         <v>0.72779804468154907</v>
       </c>
     </row>
-    <row r="94" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="s">
         <v>401</v>
       </c>
@@ -28322,7 +28319,7 @@
         <v>0.15830454230308533</v>
       </c>
     </row>
-    <row r="95" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="32" t="s">
         <v>402</v>
       </c>
@@ -28399,7 +28396,7 @@
         <v>0.28555735945701599</v>
       </c>
     </row>
-    <row r="96" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="32" t="s">
         <v>403</v>
       </c>
@@ -28476,7 +28473,7 @@
         <v>0.26823419332504272</v>
       </c>
     </row>
-    <row r="97" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
         <v>404</v>
       </c>
@@ -28553,7 +28550,7 @@
         <v>0.20041759312152863</v>
       </c>
     </row>
-    <row r="98" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
         <v>405</v>
       </c>
@@ -28630,7 +28627,7 @@
         <v>0.28437429666519165</v>
       </c>
     </row>
-    <row r="99" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="32" t="s">
         <v>406</v>
       </c>
@@ -28707,7 +28704,7 @@
         <v>0.25010630488395691</v>
       </c>
     </row>
-    <row r="100" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="32" t="s">
         <v>407</v>
       </c>
@@ -28784,7 +28781,7 @@
         <v>0.30737441778182983</v>
       </c>
     </row>
-    <row r="101" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="32" t="s">
         <v>408</v>
       </c>
@@ -28861,7 +28858,7 @@
         <v>0.50466680526733398</v>
       </c>
     </row>
-    <row r="102" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="32" t="s">
         <v>409</v>
       </c>
@@ -28938,7 +28935,7 @@
         <v>0.22827835381031036</v>
       </c>
     </row>
-    <row r="103" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="32" t="s">
         <v>410</v>
       </c>
@@ -29015,7 +29012,7 @@
         <v>0.3026200532913208</v>
       </c>
     </row>
-    <row r="104" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="32" t="s">
         <v>411</v>
       </c>
@@ -29092,7 +29089,7 @@
         <v>0.22535316646099091</v>
       </c>
     </row>
-    <row r="105" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="32" t="s">
         <v>412</v>
       </c>
@@ -29169,7 +29166,7 @@
         <v>0.2269635945558548</v>
       </c>
     </row>
-    <row r="106" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="32" t="s">
         <v>413</v>
       </c>
@@ -29246,7 +29243,7 @@
         <v>0.28848472237586975</v>
       </c>
     </row>
-    <row r="107" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="32" t="s">
         <v>414</v>
       </c>
@@ -29323,7 +29320,7 @@
         <v>0.39695122838020325</v>
       </c>
     </row>
-    <row r="108" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="32" t="s">
         <v>415</v>
       </c>
@@ -29400,7 +29397,7 @@
         <v>0.45746159553527832</v>
       </c>
     </row>
-    <row r="109" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="32" t="s">
         <v>416</v>
       </c>
@@ -29477,7 +29474,7 @@
         <v>0.37340903282165527</v>
       </c>
     </row>
-    <row r="110" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="32" t="s">
         <v>417</v>
       </c>
@@ -29554,7 +29551,7 @@
         <v>0.5086330771446228</v>
       </c>
     </row>
-    <row r="111" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="32" t="s">
         <v>418</v>
       </c>
@@ -29631,7 +29628,7 @@
         <v>0.25598442554473877</v>
       </c>
     </row>
-    <row r="112" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="32" t="s">
         <v>419</v>
       </c>
@@ -29708,7 +29705,7 @@
         <v>0.34975156188011169</v>
       </c>
     </row>
-    <row r="113" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="32" t="s">
         <v>420</v>
       </c>
@@ -29785,7 +29782,7 @@
         <v>0.27603870630264282</v>
       </c>
     </row>
-    <row r="114" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="32" t="s">
         <v>421</v>
       </c>
@@ -29862,7 +29859,7 @@
         <v>0.40216988325119019</v>
       </c>
     </row>
-    <row r="115" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="32" t="s">
         <v>422</v>
       </c>
@@ -29939,7 +29936,7 @@
         <v>0.30762571096420288</v>
       </c>
     </row>
-    <row r="116" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="32" t="s">
         <v>423</v>
       </c>
@@ -30016,7 +30013,7 @@
         <v>0.58714056015014648</v>
       </c>
     </row>
-    <row r="117" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="32" t="s">
         <v>424</v>
       </c>
@@ -30093,7 +30090,7 @@
         <v>0.44994673132896423</v>
       </c>
     </row>
-    <row r="118" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="32" t="s">
         <v>425</v>
       </c>
@@ -30170,7 +30167,7 @@
         <v>0.47607287764549255</v>
       </c>
     </row>
-    <row r="119" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="32" t="s">
         <v>426</v>
       </c>
@@ -30247,7 +30244,7 @@
         <v>0.36488872766494751</v>
       </c>
     </row>
-    <row r="120" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="32" t="s">
         <v>427</v>
       </c>
@@ -30324,7 +30321,7 @@
         <v>0.28654897212982178</v>
       </c>
     </row>
-    <row r="121" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="32" t="s">
         <v>428</v>
       </c>
@@ -30401,7 +30398,7 @@
         <v>0.34144526720046997</v>
       </c>
     </row>
-    <row r="122" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="32" t="s">
         <v>429</v>
       </c>
@@ -30478,7 +30475,7 @@
         <v>0.22241611778736115</v>
       </c>
     </row>
-    <row r="123" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="32" t="s">
         <v>430</v>
       </c>
@@ -30555,7 +30552,7 @@
         <v>0.25231030583381653</v>
       </c>
     </row>
-    <row r="124" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="32" t="s">
         <v>431</v>
       </c>
@@ -30632,7 +30629,7 @@
         <v>0.55970746278762817</v>
       </c>
     </row>
-    <row r="125" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="32" t="s">
         <v>432</v>
       </c>
@@ -30709,7 +30706,7 @@
         <v>0.26722285151481628</v>
       </c>
     </row>
-    <row r="126" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="32" t="s">
         <v>433</v>
       </c>
@@ -30786,7 +30783,7 @@
         <v>0.29379457235336304</v>
       </c>
     </row>
-    <row r="127" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="32" t="s">
         <v>434</v>
       </c>
@@ -30863,7 +30860,7 @@
         <v>0.17881979048252106</v>
       </c>
     </row>
-    <row r="128" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="32" t="s">
         <v>435</v>
       </c>
@@ -30940,7 +30937,7 @@
         <v>0.35325759649276733</v>
       </c>
     </row>
-    <row r="129" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="32" t="s">
         <v>436</v>
       </c>
@@ -31017,7 +31014,7 @@
         <v>0.15045070648193359</v>
       </c>
     </row>
-    <row r="130" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="32" t="s">
         <v>437</v>
       </c>
@@ -31094,7 +31091,7 @@
         <v>0.39486896991729736</v>
       </c>
     </row>
-    <row r="131" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="32" t="s">
         <v>438</v>
       </c>
@@ -31171,7 +31168,7 @@
         <v>0.30593407154083252</v>
       </c>
     </row>
-    <row r="132" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="32" t="s">
         <v>439</v>
       </c>
@@ -31248,7 +31245,7 @@
         <v>0.28211143612861633</v>
       </c>
     </row>
-    <row r="133" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="32" t="s">
         <v>440</v>
       </c>
@@ -31325,7 +31322,7 @@
         <v>0.41882416605949402</v>
       </c>
     </row>
-    <row r="134" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="32" t="s">
         <v>441</v>
       </c>
@@ -31402,7 +31399,7 @@
         <v>0.36238986253738403</v>
       </c>
     </row>
-    <row r="135" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="32" t="s">
         <v>442</v>
       </c>
@@ -31479,7 +31476,7 @@
         <v>0.24535337090492249</v>
       </c>
     </row>
-    <row r="136" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="32" t="s">
         <v>443</v>
       </c>
@@ -31556,7 +31553,7 @@
         <v>0.48838552832603455</v>
       </c>
     </row>
-    <row r="137" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="32" t="s">
         <v>444</v>
       </c>
@@ -31633,7 +31630,7 @@
         <v>0.30829226970672607</v>
       </c>
     </row>
-    <row r="138" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="32" t="s">
         <v>445</v>
       </c>
@@ -31710,7 +31707,7 @@
         <v>0.33618026971817017</v>
       </c>
     </row>
-    <row r="139" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="32" t="s">
         <v>446</v>
       </c>
@@ -31787,7 +31784,7 @@
         <v>0.37147349119186401</v>
       </c>
     </row>
-    <row r="140" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="32" t="s">
         <v>447</v>
       </c>
@@ -31864,7 +31861,7 @@
         <v>0.31146511435508728</v>
       </c>
     </row>
-    <row r="141" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="32" t="s">
         <v>448</v>
       </c>
@@ -31941,7 +31938,7 @@
         <v>0.43967381119728088</v>
       </c>
     </row>
-    <row r="142" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="32" t="s">
         <v>449</v>
       </c>
@@ -32018,7 +32015,7 @@
         <v>0.45340156555175781</v>
       </c>
     </row>
-    <row r="143" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="32" t="s">
         <v>450</v>
       </c>
@@ -32095,7 +32092,7 @@
         <v>0.37887352705001831</v>
       </c>
     </row>
-    <row r="144" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="32" t="s">
         <v>451</v>
       </c>
@@ -32172,7 +32169,7 @@
         <v>0.1661449521780014</v>
       </c>
     </row>
-    <row r="145" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="32" t="s">
         <v>452</v>
       </c>
@@ -32249,7 +32246,7 @@
         <v>0.23736073076725006</v>
       </c>
     </row>
-    <row r="146" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="32" t="s">
         <v>453</v>
       </c>
@@ -32326,7 +32323,7 @@
         <v>0.23682688176631927</v>
       </c>
     </row>
-    <row r="147" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="32" t="s">
         <v>454</v>
       </c>
@@ -32403,7 +32400,7 @@
         <v>0.2300117015838623</v>
       </c>
     </row>
-    <row r="148" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="32" t="s">
         <v>455</v>
       </c>
@@ -32480,7 +32477,7 @@
         <v>0.34829497337341309</v>
       </c>
     </row>
-    <row r="149" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="32" t="s">
         <v>456</v>
       </c>
@@ -32554,7 +32551,7 @@
         <v>0.29616931080818176</v>
       </c>
     </row>
-    <row r="150" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="32" t="s">
         <v>457</v>
       </c>
@@ -32631,7 +32628,7 @@
         <v>0.4630596935749054</v>
       </c>
     </row>
-    <row r="151" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="32" t="s">
         <v>458</v>
       </c>
@@ -32708,7 +32705,7 @@
         <v>0.21924585103988647</v>
       </c>
     </row>
-    <row r="152" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="32" t="s">
         <v>459</v>
       </c>
@@ -32782,7 +32779,7 @@
         <v>0.20975841581821442</v>
       </c>
     </row>
-    <row r="153" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="32" t="s">
         <v>460</v>
       </c>
@@ -32859,7 +32856,7 @@
         <v>0.18625649809837341</v>
       </c>
     </row>
-    <row r="154" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="32" t="s">
         <v>461</v>
       </c>
@@ -32933,7 +32930,7 @@
         <v>0.1283426433801651</v>
       </c>
     </row>
-    <row r="155" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="32" t="s">
         <v>462</v>
       </c>
@@ -33010,7 +33007,7 @@
         <v>0.49388605356216431</v>
       </c>
     </row>
-    <row r="156" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="32" t="s">
         <v>463</v>
       </c>
@@ -33084,7 +33081,7 @@
         <v>0.45995631814002991</v>
       </c>
     </row>
-    <row r="157" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="32" t="s">
         <v>464</v>
       </c>
@@ -33161,7 +33158,7 @@
         <v>0.35596457123756409</v>
       </c>
     </row>
-    <row r="158" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="32" t="s">
         <v>465</v>
       </c>
@@ -33238,7 +33235,7 @@
         <v>0.21581268310546875</v>
       </c>
     </row>
-    <row r="159" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="32" t="s">
         <v>466</v>
       </c>
@@ -33315,7 +33312,7 @@
         <v>0.12943816184997559</v>
       </c>
     </row>
-    <row r="160" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="32" t="s">
         <v>467</v>
       </c>
@@ -33389,7 +33386,7 @@
         <v>0.12202026695013046</v>
       </c>
     </row>
-    <row r="161" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="32" t="s">
         <v>468</v>
       </c>
@@ -33463,7 +33460,7 @@
         <v>0.184107705950737</v>
       </c>
     </row>
-    <row r="162" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="32" t="s">
         <v>469</v>
       </c>
@@ -33537,7 +33534,7 @@
         <v>0.23099616169929504</v>
       </c>
     </row>
-    <row r="163" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
         <v>470</v>
       </c>
@@ -33614,7 +33611,7 @@
         <v>0.4963763952255249</v>
       </c>
     </row>
-    <row r="164" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
         <v>471</v>
       </c>
@@ -33691,7 +33688,7 @@
         <v>0.39475861191749573</v>
       </c>
     </row>
-    <row r="165" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
         <v>472</v>
       </c>
@@ -33768,7 +33765,7 @@
         <v>0.62378960847854614</v>
       </c>
     </row>
-    <row r="166" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="32" t="s">
         <v>473</v>
       </c>
@@ -33845,7 +33842,7 @@
         <v>0.27541711926460266</v>
       </c>
     </row>
-    <row r="167" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="32" t="s">
         <v>474</v>
       </c>
@@ -33922,7 +33919,7 @@
         <v>0.63139051198959351</v>
       </c>
     </row>
-    <row r="168" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="32" t="s">
         <v>475</v>
       </c>
@@ -33999,7 +33996,7 @@
         <v>0.47367125749588013</v>
       </c>
     </row>
-    <row r="169" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="32" t="s">
         <v>476</v>
       </c>
@@ -34076,7 +34073,7 @@
         <v>0.3564155101776123</v>
       </c>
     </row>
-    <row r="170" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="32" t="s">
         <v>477</v>
       </c>
@@ -34150,7 +34147,7 @@
         <v>0.27800771594047546</v>
       </c>
     </row>
-    <row r="171" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="32" t="s">
         <v>478</v>
       </c>
@@ -34227,7 +34224,7 @@
         <v>0.44255080819129944</v>
       </c>
     </row>
-    <row r="172" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="32" t="s">
         <v>479</v>
       </c>
@@ -34304,7 +34301,7 @@
         <v>0.66277438402175903</v>
       </c>
     </row>
-    <row r="173" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="32" t="s">
         <v>480</v>
       </c>
@@ -34381,7 +34378,7 @@
         <v>0.75385189056396484</v>
       </c>
     </row>
-    <row r="174" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="32" t="s">
         <v>481</v>
       </c>
@@ -34455,7 +34452,7 @@
         <v>0.43499255180358887</v>
       </c>
     </row>
-    <row r="175" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="32" t="s">
         <v>376</v>
       </c>
@@ -34500,7 +34497,7 @@
       <c r="ED175" s="10"/>
       <c r="EE175" s="10"/>
     </row>
-    <row r="176" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="32" t="s">
         <v>376</v>
       </c>
@@ -34533,7 +34530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="32" t="s">
         <v>376</v>
       </c>
@@ -34566,7 +34563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="32" t="s">
         <v>376</v>
       </c>
@@ -34599,7 +34596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="32" t="s">
         <v>377</v>
       </c>
@@ -34632,7 +34629,7 @@
         <v>0.162337662337662</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="32" t="s">
         <v>377</v>
       </c>
@@ -34665,7 +34662,7 @@
         <v>0.23041474654377847</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="32" t="s">
         <v>377</v>
       </c>
@@ -34698,7 +34695,7 @@
         <v>0.23400936037441644</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="32" t="s">
         <v>377</v>
       </c>
@@ -34731,7 +34728,7 @@
         <v>0.15302218821729241</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="32" t="s">
         <v>377</v>
       </c>
@@ -34775,6 +34772,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100663AB788D7A8E4409C0C8F27BBECE63F" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="127f0822b766f714467baa90bfa44c3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df7f41a0-9c1e-42eb-a4a3-0247cf46dd37" xmlns:ns4="589664a6-b021-4865-b2ce-f23304a6b359" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="322b389eb35575189653dbb0f65bc017" ns3:_="" ns4:_="">
     <xsd:import namespace="df7f41a0-9c1e-42eb-a4a3-0247cf46dd37"/>
@@ -34997,36 +35009,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF54C6EA-30E2-40A7-A67A-D1B0B0300912}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B379E3D9-6878-496E-A7B4-B04196CF92A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="df7f41a0-9c1e-42eb-a4a3-0247cf46dd37"/>
-    <ds:schemaRef ds:uri="589664a6-b021-4865-b2ce-f23304a6b359"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -35049,9 +35035,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B379E3D9-6878-496E-A7B4-B04196CF92A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF54C6EA-30E2-40A7-A67A-D1B0B0300912}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="df7f41a0-9c1e-42eb-a4a3-0247cf46dd37"/>
+    <ds:schemaRef ds:uri="589664a6-b021-4865-b2ce-f23304a6b359"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>